<commit_message>
fix: upload button & data format
</commit_message>
<xml_diff>
--- a/public/student-data.xlsx
+++ b/public/student-data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sunid\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Udaan-Dummy\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{93E3A1E6-9465-4B9C-B544-BD64E4D22E78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{506609D2-8345-4E99-9E46-C9B583D82A65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="13776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Converted Sheet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>name</t>
   </si>
@@ -37,29 +37,46 @@
     <t>fees_paid</t>
   </si>
   <si>
-    <t>dropout</t>
-  </si>
-  <si>
-    <t>at_risk</t>
-  </si>
-  <si>
-    <t>backlog</t>
-  </si>
-  <si>
     <t>st_id</t>
+  </si>
+  <si>
+    <t>backlogs</t>
+  </si>
+  <si>
+    <t>Current_CGPA</t>
+  </si>
+  <si>
+    <t>branch</t>
+  </si>
+  <si>
+    <t>batch</t>
+  </si>
+  <si>
+    <t>enrolment_no</t>
+  </si>
+  <si>
+    <t>guardian_name</t>
+  </si>
+  <si>
+    <t>guardian_contact</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -70,7 +87,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -78,12 +95,46 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,47 +474,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="13" max="13" width="14.296875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="B1:I1" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>